<commit_message>
change Arctic Circle source to circumvent unexpected errors from AKBASE version
</commit_message>
<xml_diff>
--- a/data/ALL_BrokenSrc20200803_1950_working.xlsx
+++ b/data/ALL_BrokenSrc20200803_1950_working.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\updateDataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\updateDataSources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24BC7EC-A9AA-4AC9-86DE-A4566D46BC79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F47033-E4EB-4AF6-A567-5B4B3FC0B166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-72" yWindow="0" windowWidth="17544" windowHeight="16512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL_BrokenSrc20200803_1950_work" sheetId="1" r:id="rId1"/>
@@ -3051,7 +3051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3296,7 +3296,7 @@
         <v>20</v>
       </c>
       <c r="F14">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -11990,7 +11990,7 @@
         <v>569</v>
       </c>
       <c r="F550">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="551" spans="1:6" x14ac:dyDescent="0.3">
@@ -12473,7 +12473,7 @@
         <v>599</v>
       </c>
       <c r="F580">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="581" spans="1:6" x14ac:dyDescent="0.3">
@@ -12521,7 +12521,7 @@
         <v>602</v>
       </c>
       <c r="F583">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.3">
@@ -12538,7 +12538,7 @@
         <v>603</v>
       </c>
       <c r="F584">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="585" spans="1:6" x14ac:dyDescent="0.3">
@@ -12777,7 +12777,7 @@
         <v>619</v>
       </c>
       <c r="F600">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="601" spans="1:6" x14ac:dyDescent="0.3">
@@ -12825,7 +12825,7 @@
         <v>622</v>
       </c>
       <c r="F603">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="604" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add 20 FCs to sde_common
</commit_message>
<xml_diff>
--- a/data/ALL_BrokenSrc20200803_1950_working.xlsx
+++ b/data/ALL_BrokenSrc20200803_1950_working.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\updateDataSources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F47033-E4EB-4AF6-A567-5B4B3FC0B166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39CCDCA-E04D-4FED-BABA-E4F7D9EEAFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30672" yWindow="36" windowWidth="30756" windowHeight="16692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALL_BrokenSrc20200803_1950_work" sheetId="1" r:id="rId1"/>
@@ -3051,7 +3051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3168,6 +3168,9 @@
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="F6">
+        <v>223</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -3281,6 +3284,9 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F13">
+        <v>223</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -3296,7 +3302,7 @@
         <v>20</v>
       </c>
       <c r="F14">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -4184,6 +4190,9 @@
       <c r="D70" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="F70">
+        <v>208</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
@@ -4310,6 +4319,9 @@
       <c r="D79" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="F79">
+        <v>221</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
@@ -4366,6 +4378,9 @@
       <c r="D83" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="F83">
+        <v>226</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
@@ -4394,6 +4409,9 @@
       <c r="D85" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="F85">
+        <v>209</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
@@ -5692,7 +5710,9 @@
       <c r="D162" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F162" s="3"/>
+      <c r="F162" s="3">
+        <v>221</v>
+      </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163">
@@ -6086,7 +6106,9 @@
       <c r="D186" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F186" s="3"/>
+      <c r="F186" s="3">
+        <v>215</v>
+      </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187">
@@ -11756,6 +11778,9 @@
       <c r="D534" s="3" t="s">
         <v>553</v>
       </c>
+      <c r="F534">
+        <v>221</v>
+      </c>
     </row>
     <row r="535" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A535">
@@ -11787,6 +11812,9 @@
       <c r="D536" s="3" t="s">
         <v>555</v>
       </c>
+      <c r="F536">
+        <v>227</v>
+      </c>
     </row>
     <row r="537" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A537">
@@ -11801,6 +11829,9 @@
       <c r="D537" s="3" t="s">
         <v>556</v>
       </c>
+      <c r="F537">
+        <v>216</v>
+      </c>
     </row>
     <row r="538" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A538">
@@ -11930,6 +11961,9 @@
       <c r="D546" s="3" t="s">
         <v>565</v>
       </c>
+      <c r="F546">
+        <v>221</v>
+      </c>
     </row>
     <row r="547" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A547">
@@ -11990,7 +12024,7 @@
         <v>569</v>
       </c>
       <c r="F550">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="551" spans="1:6" x14ac:dyDescent="0.3">
@@ -12473,7 +12507,7 @@
         <v>599</v>
       </c>
       <c r="F580">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="581" spans="1:6" x14ac:dyDescent="0.3">
@@ -12521,7 +12555,7 @@
         <v>602</v>
       </c>
       <c r="F583">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="584" spans="1:6" x14ac:dyDescent="0.3">
@@ -12538,7 +12572,7 @@
         <v>603</v>
       </c>
       <c r="F584">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="585" spans="1:6" x14ac:dyDescent="0.3">
@@ -12777,7 +12811,7 @@
         <v>619</v>
       </c>
       <c r="F600">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="601" spans="1:6" x14ac:dyDescent="0.3">
@@ -12810,6 +12844,9 @@
       <c r="D602" s="3" t="s">
         <v>621</v>
       </c>
+      <c r="F602">
+        <v>222</v>
+      </c>
     </row>
     <row r="603" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A603">
@@ -12825,7 +12862,7 @@
         <v>622</v>
       </c>
       <c r="F603">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="604" spans="1:6" x14ac:dyDescent="0.3">
@@ -13127,6 +13164,9 @@
       <c r="D624" s="3" t="s">
         <v>643</v>
       </c>
+      <c r="F624">
+        <v>222</v>
+      </c>
     </row>
     <row r="625" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A625">
@@ -13791,6 +13831,9 @@
       </c>
       <c r="D670" s="3" t="s">
         <v>689</v>
+      </c>
+      <c r="F670">
+        <v>221</v>
       </c>
     </row>
     <row r="671" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>